<commit_message>
a little bit update
</commit_message>
<xml_diff>
--- a/backend/assets/template-peserta.xlsx
+++ b/backend/assets/template-peserta.xlsx
@@ -397,14 +397,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="30.83203125" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="30.83203125" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -412,9 +414,15 @@
         <v>Nama</v>
       </c>
       <c r="B1" t="str">
+        <v>Email</v>
+      </c>
+      <c r="C1" t="str">
+        <v>NoTelp</v>
+      </c>
+      <c r="D1" t="str">
         <v>Aktivitas</v>
       </c>
-      <c r="C1" t="str">
+      <c r="E1" t="str">
         <v>Batch</v>
       </c>
     </row>
@@ -423,9 +431,15 @@
         <v>Budi Santoso</v>
       </c>
       <c r="B2" t="str">
+        <v>budi.santoso@email.com</v>
+      </c>
+      <c r="C2" t="str">
+        <v>081234567890</v>
+      </c>
+      <c r="D2" t="str">
         <v>Try Out CPNS 2025</v>
       </c>
-      <c r="C2" t="str">
+      <c r="E2" t="str">
         <v>VII</v>
       </c>
     </row>
@@ -434,15 +448,38 @@
         <v>Siti Aminah</v>
       </c>
       <c r="B3" t="str">
+        <v>siti.aminah@email.com</v>
+      </c>
+      <c r="C3" t="str">
+        <v>081234567891</v>
+      </c>
+      <c r="D3" t="str">
         <v>Seminar Digital Marketing</v>
       </c>
-      <c r="C3" t="str">
+      <c r="E3" t="str">
         <v>I</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Ahmad Rizki</v>
+      </c>
+      <c r="B4" t="str">
+        <v>ahmad.rizki@email.com</v>
+      </c>
+      <c r="C4" t="str">
+        <v>-</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Workshop Design Thinking</v>
+      </c>
+      <c r="E4" t="str">
+        <v>III</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>